<commit_message>
Updated test data for TC50946,53557
</commit_message>
<xml_diff>
--- a/Test Data/TC_53557_Verify_DC_Unit_For_Multiple_Built_In_Non_Built_In_Isolator_Devices_Integral_Non_Integral_LED_of_FIM.xlsx
+++ b/Test Data/TC_53557_Verify_DC_Unit_For_Multiple_Built_In_Non_Built_In_Isolator_Devices_Integral_Non_Integral_LED_of_FIM.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01EC4C5-9B07-4063-9F76-31D74EB9EB07}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Devices" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -129,7 +128,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -521,11 +520,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,7 +658,7 @@
         <v>22</v>
       </c>
       <c r="J8" s="6">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -691,7 +690,7 @@
         <v>28</v>
       </c>
       <c r="J9" s="6">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>